<commit_message>
Ran DDE model without diurnal variation
</commit_message>
<xml_diff>
--- a/Model results Tmax.xlsx
+++ b/Model results Tmax.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11222"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A622359-2782-784C-A628-A09AE7CDBA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849DE678-D1B8-9640-839B-3678DAABDB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
   <si>
     <t>Species</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Bemisia argentifollii US Homestead</t>
   </si>
   <si>
-    <t>Rhopalosiphum rufiabdominalis US Naples</t>
-  </si>
-  <si>
     <t>Aphis nasturtii US Weston</t>
   </si>
   <si>
@@ -176,7 +173,13 @@
     <t>Diaphorina citri US Weston</t>
   </si>
   <si>
-    <t>No time series data b/c extinct</t>
+    <t>Rhopalosiphum rufiabdominalis US Weston</t>
+  </si>
+  <si>
+    <t>Including overwintering; no future time series data b/c extinct</t>
+  </si>
+  <si>
+    <t>Including overwintering; DDE model run for 15 years for historical period; no future time series data b/c extinct</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1049,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1701,7 +1704,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B19">
         <v>26.14</v>
@@ -1722,7 +1725,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="H19">
-        <v>1.37E-2</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="0"/>
@@ -1730,15 +1733,15 @@
       </c>
       <c r="J19" s="1">
         <f t="shared" si="1"/>
-        <v>-0.23888888888888882</v>
+        <v>-1</v>
       </c>
       <c r="K19" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>26.14</v>
@@ -1775,7 +1778,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21">
         <v>26.24</v>
@@ -1812,7 +1815,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>30.9</v>
@@ -1849,7 +1852,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23">
         <v>42.81</v>
@@ -1881,7 +1884,7 @@
         <v>-1</v>
       </c>
       <c r="K23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1918,12 +1921,12 @@
         <v>-0.10339943342776198</v>
       </c>
       <c r="K24" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>35.270000000000003</v>
@@ -1960,7 +1963,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>36.07</v>
@@ -1997,7 +2000,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27">
         <v>42.42</v>
@@ -2029,12 +2032,12 @@
         <v>-2.1276595744680906E-2</v>
       </c>
       <c r="K27" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28">
         <v>38.93</v>
@@ -2066,12 +2069,12 @@
         <v>-0.14285714285714293</v>
       </c>
       <c r="K28" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29">
         <v>38.93</v>
@@ -2103,12 +2106,12 @@
         <v>-0.27272727272727265</v>
       </c>
       <c r="K29" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30">
         <v>38.93</v>

</xml_diff>

<commit_message>
Fixed several errors in calculating r in "Intrinsic growth rate.R"
</commit_message>
<xml_diff>
--- a/Model results Tmax.xlsx
+++ b/Model results Tmax.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849DE678-D1B8-9640-839B-3678DAABDB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1967CA-EA26-3840-87EA-E70132E1397F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
   <si>
     <t>Species</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Including overwintering; DDE model run for 15 years for historical period; no future time series data b/c extinct</t>
+  </si>
+  <si>
+    <t>Extinct in model</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,6 +333,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -679,18 +688,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1049,7 +1056,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,25 +1114,28 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="F2" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G2">
-        <v>4.58E-2</v>
-      </c>
-      <c r="H2">
-        <v>3.09E-2</v>
+      <c r="E2" s="6">
+        <v>0.105</v>
+      </c>
+      <c r="F2" s="7">
+        <v>3.1E-2</v>
+      </c>
+      <c r="G2" s="6">
+        <v>7.8E-2</v>
+      </c>
+      <c r="H2" s="6">
+        <v>-2E-3</v>
       </c>
       <c r="I2" s="1">
-        <f>MAX((F2-E2)/E2,-1)</f>
-        <v>-0.25742574257425749</v>
+        <f>(F2-E2)/E2</f>
+        <v>-0.7047619047619047</v>
       </c>
       <c r="J2" s="1">
-        <f>MAX((H2-G2)/G2,-1)</f>
-        <v>-0.32532751091703055</v>
+        <f>(H2-G2)/G2</f>
+        <v>-1.0256410256410258</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1141,25 +1151,25 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1">
-        <v>0.09</v>
-      </c>
-      <c r="F3">
-        <v>0.151</v>
-      </c>
-      <c r="G3">
-        <v>2.6599999999999999E-2</v>
-      </c>
-      <c r="H3">
-        <v>3.1199999999999999E-2</v>
+      <c r="E3" s="7">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.114</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.14099999999999999</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I30" si="0">MAX((F3-E3)/E3,-1)</f>
-        <v>0.67777777777777781</v>
+        <f t="shared" ref="I3:I30" si="0">(F3-E3)/E3</f>
+        <v>-2.6845637583892641E-2</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J30" si="1">MAX((H3-G3)/G3,-1)</f>
-        <v>0.17293233082706769</v>
+        <f t="shared" ref="J3:J30" si="1">(H3-G3)/G3</f>
+        <v>0.23684210526315774</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -1175,25 +1185,25 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="G4">
-        <v>1.52</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1.76</v>
+      <c r="E4" s="7">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.104</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>0.55681818181818199</v>
+        <v>-0.28767123287671231</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="1"/>
-        <v>0.15789473684210525</v>
+        <v>-0.69852941176470584</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -1209,25 +1219,28 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="G5" s="4">
-        <v>3.0099999999999998E-2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>2.23E-2</v>
+      <c r="E5" s="6">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F5" s="7">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="H5" s="7">
+        <v>-3.6999999999999998E-2</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>1.5833333333333335</v>
+        <v>-0.18811881188118815</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>-0.25913621262458464</v>
+        <v>-1.2151162790697674</v>
+      </c>
+      <c r="K5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1243,25 +1256,25 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="G6">
-        <v>4.8999999999999998E-3</v>
-      </c>
-      <c r="H6">
-        <v>4.1999999999999997E-3</v>
+      <c r="E6" s="7">
+        <v>0.113</v>
+      </c>
+      <c r="F6" s="7">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="H6" s="7">
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>-0.52941176470588236</v>
+        <v>-1.6194690265486724</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="1"/>
-        <v>-0.14285714285714288</v>
+        <v>-0.57971014492753625</v>
       </c>
       <c r="K6" t="s">
         <v>27</v>
@@ -1280,25 +1293,25 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="G7">
-        <v>5.8999999999999999E-3</v>
-      </c>
-      <c r="H7">
-        <v>5.5999999999999999E-3</v>
+      <c r="E7" s="7">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G7" s="6">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.03</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>8.1632653061224414E-2</v>
+        <v>-1.9607843137254784E-2</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>-5.0847457627118633E-2</v>
+        <v>-0.49152542372881353</v>
       </c>
       <c r="K7" t="s">
         <v>27</v>
@@ -1317,25 +1330,25 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8">
-        <v>0.104</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="G8">
-        <v>4.8999999999999998E-3</v>
-      </c>
-      <c r="H8">
-        <v>5.8999999999999999E-3</v>
+      <c r="E8" s="6">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="F8" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G8" s="6">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H8" s="6">
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>-2.884615384615374E-2</v>
+        <v>-0.62184873949579833</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="1"/>
-        <v>0.20408163265306123</v>
+        <v>-0.27999999999999997</v>
       </c>
       <c r="K8" t="s">
         <v>27</v>
@@ -1354,25 +1367,25 @@
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="G9">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="H9">
-        <v>5.4000000000000003E-3</v>
+      <c r="E9" s="7">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="H9" s="6">
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.20370370370370375</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="1"/>
-        <v>-1.8181818181818073E-2</v>
+        <v>-0.50877192982456143</v>
       </c>
       <c r="K9" t="s">
         <v>27</v>
@@ -1391,25 +1404,25 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="1">
-        <v>0.188</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.193</v>
-      </c>
-      <c r="G10" s="5">
-        <v>2.1600000000000001E-2</v>
-      </c>
-      <c r="H10" s="5">
-        <v>2.1899999999999999E-2</v>
+      <c r="E10" s="7">
+        <v>0.186</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.14599999999999999</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>2.6595744680851088E-2</v>
+        <v>-0.35483870967741937</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="1"/>
-        <v>1.3888888888888805E-2</v>
+        <v>-0.61679790026246717</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1425,25 +1438,29 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="10">
-        <v>0.18</v>
-      </c>
-      <c r="F11" s="10">
-        <v>0.155</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0.36099999999999999</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="I11" s="10">
-        <f t="shared" si="0"/>
-        <v>-0.13888888888888887</v>
+      <c r="E11" s="7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F11" s="7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="H11" s="8">
+        <f>-1.62</f>
+        <v>-1.62</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.94202898550724634</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="1"/>
-        <v>8.3102493074792325E-2</v>
+        <f>(H11-G11)/G11</f>
+        <v>-9.3505154639175263</v>
+      </c>
+      <c r="K11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1459,25 +1476,25 @@
       <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E12">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.153</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H12">
-        <v>2.7799999999999998E-2</v>
+      <c r="E12" s="6">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="F12" s="7">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.53</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.159</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.12068965517241374</v>
+        <v>-0.95104895104895104</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="1"/>
-        <v>0.11199999999999988</v>
+        <v>-0.7</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1499,7 +1516,7 @@
       <c r="F13" s="1">
         <v>2.4E-2</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="H13">
@@ -1536,7 +1553,7 @@
       <c r="F14" s="1">
         <v>-1.9E-2</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>8.3000000000000001E-3</v>
       </c>
       <c r="H14">
@@ -1544,7 +1561,7 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-1.3220338983050848</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="1"/>
@@ -1573,7 +1590,7 @@
       <c r="F15" s="1">
         <v>0.189</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H15">
@@ -1610,7 +1627,7 @@
       <c r="F16" s="1">
         <v>0.216</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>3.3E-3</v>
       </c>
       <c r="H16">
@@ -1647,7 +1664,7 @@
       <c r="F17" s="1">
         <v>0.154</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>1.9699999999999999E-2</v>
       </c>
       <c r="H17">
@@ -1684,7 +1701,7 @@
       <c r="F18" s="1">
         <v>0.17399999999999999</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>3.8600000000000002E-2</v>
       </c>
       <c r="H18">
@@ -1721,7 +1738,7 @@
       <c r="F19" s="1">
         <v>0.315</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="H19">
@@ -1758,7 +1775,7 @@
       <c r="F20" s="1">
         <v>0.26800000000000002</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>1.46E-2</v>
       </c>
       <c r="H20" s="2">
@@ -1795,7 +1812,7 @@
       <c r="F21" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>6.7199999999999996E-2</v>
       </c>
       <c r="H21">
@@ -1832,7 +1849,7 @@
       <c r="F22" s="1">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>2.0199999999999999E-2</v>
       </c>
       <c r="H22">
@@ -1863,25 +1880,25 @@
       <c r="D23" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="4">
         <v>0.188</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="4">
         <v>0.496</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="4">
         <v>1.1200000000000001</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="5">
         <v>-2.3E-2</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="1">
         <f t="shared" si="0"/>
         <v>1.6382978723404256</v>
       </c>
-      <c r="J23" s="7">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+      <c r="J23" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.0205357142857141</v>
       </c>
       <c r="K23" t="s">
         <v>45</v>
@@ -1906,7 +1923,7 @@
       <c r="F24" s="1">
         <v>0.86199999999999999</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>7.06</v>
       </c>
       <c r="H24">
@@ -1943,7 +1960,7 @@
       <c r="F25" s="1">
         <v>0.20799999999999999</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>7.1999999999999998E-3</v>
       </c>
       <c r="H25">
@@ -1980,7 +1997,7 @@
       <c r="F26" s="1">
         <v>0.20499999999999999</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="H26">
@@ -2017,7 +2034,7 @@
       <c r="F27" s="1">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="H27">
@@ -2054,7 +2071,7 @@
       <c r="F28" s="1">
         <v>-0.248</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="H28">
@@ -2062,7 +2079,7 @@
       </c>
       <c r="I28" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-6.9047619047619042</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" si="1"/>
@@ -2091,7 +2108,7 @@
       <c r="F29" s="1">
         <v>-0.26600000000000001</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="H29">
@@ -2099,7 +2116,7 @@
       </c>
       <c r="I29" s="1">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>-3.078125</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" si="1"/>
@@ -2128,7 +2145,7 @@
       <c r="F30" s="1">
         <v>0.11700000000000001</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="H30" s="1">

</xml_diff>

<commit_message>
Calculated r without diurnal variation for remainder of species
</commit_message>
<xml_diff>
--- a/Model results Tmax.xlsx
+++ b/Model results Tmax.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1967CA-EA26-3840-87EA-E70132E1397F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383DC696-72BD-9F48-99F7-B024EEF92571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,13 +176,13 @@
     <t>Rhopalosiphum rufiabdominalis US Weston</t>
   </si>
   <si>
-    <t>Including overwintering; no future time series data b/c extinct</t>
-  </si>
-  <si>
-    <t>Including overwintering; DDE model run for 15 years for historical period; no future time series data b/c extinct</t>
-  </si>
-  <si>
     <t>Extinct in model</t>
+  </si>
+  <si>
+    <t>Including overwintering; no future time series data b/c extinct; estimated r in future model using -dA[T]</t>
+  </si>
+  <si>
+    <t>Including overwintering; DDE model run for 15 years for historical period; no future time series data b/c extinct; estimated r in future model using -dA[T]</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -341,7 +341,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -519,12 +519,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -688,16 +682,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1053,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,28 +1109,28 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>0.105</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>7.8E-2</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>-2E-3</v>
       </c>
       <c r="I2" s="1">
         <f>(F2-E2)/E2</f>
         <v>-0.7047619047619047</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="8">
         <f>(H2-G2)/G2</f>
         <v>-1.0256410256410258</v>
       </c>
       <c r="K2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1151,16 +1146,16 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>0.14899999999999999</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>0.14499999999999999</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>0.114</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>0.14099999999999999</v>
       </c>
       <c r="I3" s="1">
@@ -1185,16 +1180,16 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>0.14599999999999999</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>0.104</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>0.13600000000000001</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="I4" s="1">
@@ -1219,28 +1214,28 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.10100000000000001</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <v>0.17199999999999999</v>
       </c>
-      <c r="H5" s="7">
-        <v>-3.6999999999999998E-2</v>
+      <c r="H5" s="6">
+        <v>-4.2999999999999997E-2</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
         <v>-0.18811881188118815</v>
       </c>
-      <c r="J5" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.2151162790697674</v>
+      <c r="J5" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.25</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -1256,16 +1251,16 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>0.113</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="I6" s="1">
@@ -1293,16 +1288,16 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>0.05</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>0.03</v>
       </c>
       <c r="I7" s="1">
@@ -1330,16 +1325,16 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>0.11899999999999999</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="I8" s="1">
@@ -1367,16 +1362,16 @@
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="I9" s="1">
@@ -1404,16 +1399,16 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>0.186</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>0.12</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>0.38100000000000001</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>0.14599999999999999</v>
       </c>
       <c r="I10" s="1">
@@ -1438,16 +1433,16 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>0.13800000000000001</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>0.19400000000000001</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <f>-1.62</f>
         <v>-1.62</v>
       </c>
@@ -1455,12 +1450,12 @@
         <f t="shared" si="0"/>
         <v>-0.94202898550724634</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="8">
         <f>(H11-G11)/G11</f>
         <v>-9.3505154639175263</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1476,16 +1471,16 @@
       <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>0.14299999999999999</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>0.53</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>0.159</v>
       </c>
       <c r="I12" s="1">
@@ -1511,27 +1506,27 @@
         <v>11</v>
       </c>
       <c r="E13" s="1">
-        <v>6.0999999999999999E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F13" s="1">
-        <v>2.4E-2</v>
+        <v>-2.5999999999999999E-2</v>
       </c>
       <c r="G13" s="1">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-1.7999999999999999E-2</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>-0.60655737704918034</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-1.4333333333333333</v>
+      </c>
+      <c r="J13" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.2686567164179106</v>
       </c>
       <c r="K13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1548,27 +1543,27 @@
         <v>11</v>
       </c>
       <c r="E14" s="1">
-        <v>5.8999999999999997E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>-1.9E-2</v>
+        <v>-0.125</v>
       </c>
       <c r="G14" s="1">
-        <v>8.3000000000000001E-3</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H14" s="4">
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>-1.3220338983050848</v>
-      </c>
-      <c r="J14" s="1">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-3.4038461538461537</v>
+      </c>
+      <c r="J14" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.3055555555555556</v>
       </c>
       <c r="K14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1585,27 +1580,27 @@
         <v>20</v>
       </c>
       <c r="E15" s="1">
-        <v>0.23499999999999999</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="F15" s="1">
-        <v>0.189</v>
+        <v>0.11</v>
       </c>
       <c r="G15" s="1">
-        <v>5.0000000000000001E-3</v>
+        <v>7.8E-2</v>
       </c>
       <c r="H15">
-        <v>6.7000000000000002E-3</v>
+        <v>-5.5E-2</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="0"/>
-        <v>-0.19574468085106378</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="1"/>
-        <v>0.34</v>
+        <v>-0.52991452991452992</v>
+      </c>
+      <c r="J15" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.7051282051282053</v>
       </c>
       <c r="K15" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1622,31 +1617,31 @@
         <v>20</v>
       </c>
       <c r="E16" s="1">
-        <v>0.24</v>
+        <v>0.253</v>
       </c>
       <c r="F16" s="1">
-        <v>0.216</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="G16" s="1">
-        <v>3.3E-3</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="H16">
-        <v>4.8999999999999998E-3</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="I16" s="1">
         <f t="shared" si="0"/>
-        <v>-9.9999999999999978E-2</v>
+        <v>-0.35968379446640314</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="1"/>
-        <v>0.48484848484848481</v>
+        <v>-0.21126760563380273</v>
       </c>
       <c r="K16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B17">
@@ -1659,31 +1654,31 @@
         <v>20</v>
       </c>
       <c r="E17" s="1">
-        <v>0.12</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="F17" s="1">
-        <v>0.154</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="G17" s="1">
-        <v>1.9699999999999999E-2</v>
+        <v>0.106</v>
       </c>
       <c r="H17">
-        <v>1.2500000000000001E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="0"/>
-        <v>0.28333333333333338</v>
+        <v>0.1676646706586826</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="1"/>
-        <v>-0.365482233502538</v>
+        <v>-0.169811320754717</v>
       </c>
       <c r="K17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B18">
@@ -1696,31 +1691,31 @@
         <v>20</v>
       </c>
       <c r="E18" s="1">
-        <v>0.14399999999999999</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="F18" s="1">
-        <v>0.17399999999999999</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="G18" s="1">
-        <v>3.8600000000000002E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="H18">
-        <v>3.9100000000000003E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="I18" s="1">
         <f t="shared" si="0"/>
-        <v>0.20833333333333334</v>
+        <v>1.8404907975460138E-2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="1"/>
-        <v>1.295336787564768E-2</v>
+        <v>0.19736842105263158</v>
       </c>
       <c r="K18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B19">
@@ -1736,28 +1731,28 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="F19" s="1">
-        <v>0.315</v>
+        <v>0.34</v>
       </c>
       <c r="G19" s="1">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H19" s="4">
+        <v>-0.10199999999999999</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="0"/>
-        <v>-8.6956521739130363E-2</v>
-      </c>
-      <c r="J19" s="1">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+        <v>-1.4492753623188259E-2</v>
+      </c>
+      <c r="J19" s="8">
+        <f t="shared" si="1"/>
+        <v>-5.6363636363636367</v>
       </c>
       <c r="K19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B20">
@@ -1770,31 +1765,31 @@
         <v>20</v>
       </c>
       <c r="E20" s="1">
-        <v>0.247</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="F20" s="1">
-        <v>0.26800000000000002</v>
+        <v>0.252</v>
       </c>
       <c r="G20" s="1">
-        <v>1.46E-2</v>
-      </c>
-      <c r="H20" s="2">
-        <v>1.4E-2</v>
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.18</v>
       </c>
       <c r="I20" s="1">
         <f t="shared" si="0"/>
-        <v>8.5020242914979838E-2</v>
+        <v>-2.3255813953488393E-2</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="1"/>
-        <v>-4.1095890410958895E-2</v>
+        <v>7.1428571428571327E-2</v>
       </c>
       <c r="K20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B21">
@@ -1807,31 +1802,31 @@
         <v>20</v>
       </c>
       <c r="E21" s="1">
-        <v>9.0999999999999998E-2</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="F21" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="G21" s="1">
-        <v>6.7199999999999996E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="H21">
-        <v>7.4499999999999997E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" si="0"/>
-        <v>-0.75824175824175832</v>
+        <v>-0.1931818181818182</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="1"/>
-        <v>0.1086309523809524</v>
+        <v>5.1948051948051993E-2</v>
       </c>
       <c r="K21" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B22">
@@ -1844,27 +1839,27 @@
         <v>20</v>
       </c>
       <c r="E22" s="1">
-        <v>0.122</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F22" s="1">
-        <v>7.2999999999999995E-2</v>
+        <v>-0.42</v>
       </c>
       <c r="G22" s="1">
-        <v>2.0199999999999999E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="H22">
-        <v>1.8599999999999998E-2</v>
+        <v>-0.123</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="0"/>
-        <v>-0.40163934426229508</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" si="1"/>
-        <v>-7.9207920792079251E-2</v>
+        <v>-8.3684210526315788</v>
+      </c>
+      <c r="J22" s="8">
+        <f t="shared" si="1"/>
+        <v>-4.2368421052631584</v>
       </c>
       <c r="K22" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1880,25 +1875,25 @@
       <c r="D23" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="4">
-        <v>0.188</v>
-      </c>
-      <c r="F23" s="4">
-        <v>0.496</v>
-      </c>
-      <c r="G23" s="4">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="H23" s="5">
-        <v>-2.3E-2</v>
+      <c r="E23" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="F23" s="3">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="H23" s="4">
+        <v>-5.3999999999999999E-2</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
-        <v>1.6382978723404256</v>
-      </c>
-      <c r="J23" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.0205357142857141</v>
+        <v>-0.8935483870967742</v>
+      </c>
+      <c r="J23" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.0534653465346535</v>
       </c>
       <c r="K23" t="s">
         <v>45</v>
@@ -1917,32 +1912,32 @@
       <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="1">
-        <v>1.67</v>
+      <c r="E24" s="8">
+        <v>1.61</v>
       </c>
       <c r="F24" s="1">
-        <v>0.86199999999999999</v>
+        <v>-0.49199999999999999</v>
       </c>
       <c r="G24" s="1">
-        <v>7.06</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="H24">
-        <v>6.33</v>
+        <v>-0.42299999999999999</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="0"/>
-        <v>-0.48383233532934128</v>
-      </c>
-      <c r="J24" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.10339943342776198</v>
+        <v>-1.3055900621118013</v>
+      </c>
+      <c r="J24" s="8">
+        <f t="shared" si="1"/>
+        <v>-2.5053380782918144</v>
       </c>
       <c r="K24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B25">
@@ -1955,31 +1950,31 @@
         <v>20</v>
       </c>
       <c r="E25" s="1">
-        <v>0.222</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="F25" s="1">
-        <v>0.20799999999999999</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="G25" s="1">
-        <v>7.1999999999999998E-3</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H25">
-        <v>9.9000000000000008E-3</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="0"/>
-        <v>-6.3063063063063113E-2</v>
+        <v>-0.83333333333333326</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="1"/>
-        <v>0.37500000000000017</v>
+        <v>-1.4598540145985413E-2</v>
       </c>
       <c r="K25" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B26">
@@ -1992,31 +1987,31 @@
         <v>20</v>
       </c>
       <c r="E26" s="1">
-        <v>0.221</v>
+        <v>0.21</v>
       </c>
       <c r="F26" s="1">
-        <v>0.20499999999999999</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="G26" s="1">
-        <v>4.8999999999999998E-3</v>
+        <v>0.122</v>
       </c>
       <c r="H26">
-        <v>5.3E-3</v>
+        <v>0.104</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="0"/>
-        <v>-7.2398190045248931E-2</v>
+        <v>-0.29523809523809524</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="1"/>
-        <v>8.1632653061224525E-2</v>
+        <v>-0.1475409836065574</v>
       </c>
       <c r="K26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B27">
@@ -2029,31 +2024,31 @@
         <v>20</v>
       </c>
       <c r="E27" s="1">
-        <v>0.23799999999999999</v>
+        <v>0.26700000000000002</v>
       </c>
       <c r="F27" s="1">
-        <v>3.5000000000000003E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="G27" s="1">
-        <v>4.7000000000000002E-3</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="H27">
-        <v>4.5999999999999999E-3</v>
+        <v>-4.1000000000000002E-2</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="0"/>
-        <v>-0.8529411764705882</v>
-      </c>
-      <c r="J27" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.1276595744680906E-2</v>
+        <v>-0.82397003745318353</v>
+      </c>
+      <c r="J27" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.231638418079096</v>
       </c>
       <c r="K27" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B28">
@@ -2066,31 +2061,31 @@
         <v>20</v>
       </c>
       <c r="E28" s="1">
-        <v>4.2000000000000003E-2</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="F28" s="1">
-        <v>-0.248</v>
+        <v>-0.52800000000000002</v>
       </c>
       <c r="G28" s="1">
-        <v>6.9999999999999999E-4</v>
+        <v>1.4E-2</v>
       </c>
       <c r="H28">
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="I28" s="1">
-        <f t="shared" si="0"/>
-        <v>-6.9047619047619042</v>
-      </c>
-      <c r="J28" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.14285714285714293</v>
+        <v>-4.9000000000000002E-2</v>
+      </c>
+      <c r="I28" s="9">
+        <f>(F28-E28)/ABS(E28)</f>
+        <v>-11.000000000000002</v>
+      </c>
+      <c r="J28" s="8">
+        <f t="shared" si="1"/>
+        <v>-4.5</v>
       </c>
       <c r="K28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B29">
@@ -2103,31 +2098,31 @@
         <v>20</v>
       </c>
       <c r="E29" s="1">
-        <v>0.128</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F29" s="1">
-        <v>-0.26600000000000001</v>
+        <v>-0.67100000000000004</v>
       </c>
       <c r="G29" s="1">
-        <v>1.0999999999999999E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="H29">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="I29" s="1">
-        <f t="shared" si="0"/>
-        <v>-3.078125</v>
-      </c>
-      <c r="J29" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.27272727272727265</v>
+        <v>-6.2E-2</v>
+      </c>
+      <c r="I29" s="9">
+        <f t="shared" si="0"/>
+        <v>-28.958333333333336</v>
+      </c>
+      <c r="J29" s="8">
+        <f t="shared" si="1"/>
+        <v>-1.6458333333333333</v>
       </c>
       <c r="K29" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B30">
@@ -2140,30 +2135,36 @@
         <v>20</v>
       </c>
       <c r="E30" s="1">
-        <v>0.19</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="F30" s="1">
-        <v>0.11700000000000001</v>
+        <v>1.9E-2</v>
       </c>
       <c r="G30" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>0.112</v>
       </c>
       <c r="H30" s="1">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="0"/>
-        <v>-0.38421052631578945</v>
+        <v>-0.88622754491017974</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="1"/>
-        <v>-0.33333333333333331</v>
+        <v>-0.5535714285714286</v>
       </c>
       <c r="K30" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F32" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="I28" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ran statistical analyses for daily max temperature case
</commit_message>
<xml_diff>
--- a/Model results Tmax.xlsx
+++ b/Model results Tmax.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383DC696-72BD-9F48-99F7-B024EEF92571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24D8B7F-24BD-544F-A78B-17F0E1C179A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t>Species</t>
   </si>
@@ -183,15 +183,20 @@
   </si>
   <si>
     <t>Including overwintering; DDE model run for 15 years for historical period; no future time series data b/c extinct; estimated r in future model using -dA[T]</t>
+  </si>
+  <si>
+    <t>delta.prop.TPC</t>
+  </si>
+  <si>
+    <t>delta.prop.model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -682,7 +687,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -692,7 +697,6 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1048,20 +1052,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1093,10 +1097,16 @@
         <v>29</v>
       </c>
       <c r="K1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1122,18 +1132,26 @@
         <v>-2E-3</v>
       </c>
       <c r="I2" s="1">
+        <f>F2-E2</f>
+        <v>-7.3999999999999996E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <f>H2-G2</f>
+        <v>-0.08</v>
+      </c>
+      <c r="K2" s="1">
         <f>(F2-E2)/E2</f>
         <v>-0.7047619047619047</v>
       </c>
-      <c r="J2" s="8">
+      <c r="L2" s="1">
         <f>(H2-G2)/G2</f>
         <v>-1.0256410256410258</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1159,15 +1177,23 @@
         <v>0.14099999999999999</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I30" si="0">(F3-E3)/E3</f>
+        <f t="shared" ref="I3:I30" si="0">F3-E3</f>
+        <v>-4.0000000000000036E-3</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J30" si="1">H3-G3</f>
+        <v>2.6999999999999982E-2</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K30" si="2">(F3-E3)/E3</f>
         <v>-2.6845637583892641E-2</v>
       </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J30" si="1">(H3-G3)/G3</f>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L30" si="3">(H3-G3)/G3</f>
         <v>0.23684210526315774</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1194,14 +1220,22 @@
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
+        <v>-4.1999999999999996E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>-9.5000000000000001E-2</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="2"/>
         <v>-0.28767123287671231</v>
       </c>
-      <c r="J4" s="1">
-        <f t="shared" si="1"/>
+      <c r="L4" s="1">
+        <f t="shared" si="3"/>
         <v>-0.69852941176470584</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1228,17 +1262,25 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
+        <v>-1.9000000000000003E-2</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.21499999999999997</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="2"/>
         <v>-0.18811881188118815</v>
       </c>
-      <c r="J5" s="8">
-        <f t="shared" si="1"/>
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
         <v>-1.25</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1265,17 +1307,25 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
+        <v>-0.183</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>-4.0000000000000008E-2</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="2"/>
         <v>-1.6194690265486724</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" si="1"/>
+      <c r="L6" s="1">
+        <f t="shared" si="3"/>
         <v>-0.57971014492753625</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1302,17 +1352,25 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
+        <v>-9.9999999999999395E-4</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.8999999999999998E-2</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="2"/>
         <v>-1.9607843137254784E-2</v>
       </c>
-      <c r="J7" s="1">
-        <f t="shared" si="1"/>
+      <c r="L7" s="1">
+        <f t="shared" si="3"/>
         <v>-0.49152542372881353</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1339,17 +1397,25 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
+        <v>-7.3999999999999996E-2</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.0999999999999998E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="2"/>
         <v>-0.62184873949579833</v>
       </c>
-      <c r="J8" s="1">
-        <f t="shared" si="1"/>
+      <c r="L8" s="1">
+        <f t="shared" si="3"/>
         <v>-0.27999999999999997</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1376,17 +1442,25 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
+        <v>-1.1000000000000003E-2</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="2"/>
         <v>-0.20370370370370375</v>
       </c>
-      <c r="J9" s="1">
-        <f t="shared" si="1"/>
+      <c r="L9" s="1">
+        <f t="shared" si="3"/>
         <v>-0.50877192982456143</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1413,14 +1487,22 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
+        <v>-6.6000000000000003E-2</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.23500000000000001</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="2"/>
         <v>-0.35483870967741937</v>
       </c>
-      <c r="J10" s="1">
-        <f t="shared" si="1"/>
+      <c r="L10" s="1">
+        <f t="shared" si="3"/>
         <v>-0.61679790026246717</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1448,17 +1530,25 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
+        <v>-0.13</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.8140000000000001</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="2"/>
         <v>-0.94202898550724634</v>
       </c>
-      <c r="J11" s="8">
-        <f>(H11-G11)/G11</f>
+      <c r="L11" s="1">
+        <f t="shared" si="3"/>
         <v>-9.3505154639175263</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1485,14 +1575,22 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
+        <v>-0.13599999999999998</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.371</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="2"/>
         <v>-0.95104895104895104</v>
       </c>
-      <c r="J12" s="1">
-        <f t="shared" si="1"/>
+      <c r="L12" s="1">
+        <f t="shared" si="3"/>
         <v>-0.7</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1519,17 +1617,25 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
+        <v>-8.5999999999999993E-2</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="1"/>
+        <v>-8.5000000000000006E-2</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="2"/>
         <v>-1.4333333333333333</v>
       </c>
-      <c r="J13" s="8">
-        <f t="shared" si="1"/>
+      <c r="L13" s="1">
+        <f t="shared" si="3"/>
         <v>-1.2686567164179106</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1556,17 +1662,25 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
+        <v>-0.17699999999999999</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="1"/>
+        <v>-9.4E-2</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="2"/>
         <v>-3.4038461538461537</v>
       </c>
-      <c r="J14" s="8">
-        <f t="shared" si="1"/>
+      <c r="L14" s="1">
+        <f t="shared" si="3"/>
         <v>-1.3055555555555556</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1593,17 +1707,25 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" si="0"/>
+        <v>-0.12400000000000001</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.13300000000000001</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="2"/>
         <v>-0.52991452991452992</v>
       </c>
-      <c r="J15" s="8">
-        <f t="shared" si="1"/>
+      <c r="L15" s="1">
+        <f t="shared" si="3"/>
         <v>-1.7051282051282053</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1630,17 +1752,25 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" si="0"/>
+        <v>-9.0999999999999998E-2</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.4999999999999993E-2</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="2"/>
         <v>-0.35968379446640314</v>
       </c>
-      <c r="J16" s="1">
-        <f t="shared" si="1"/>
+      <c r="L16" s="1">
+        <f t="shared" si="3"/>
         <v>-0.21126760563380273</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
@@ -1667,17 +1797,25 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" si="0"/>
+        <v>2.7999999999999997E-2</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.8000000000000002E-2</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="2"/>
         <v>0.1676646706586826</v>
       </c>
-      <c r="J17" s="1">
-        <f t="shared" si="1"/>
+      <c r="L17" s="1">
+        <f t="shared" si="3"/>
         <v>-0.169811320754717</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -1704,17 +1842,25 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" si="0"/>
+        <v>3.0000000000000027E-3</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="2"/>
         <v>1.8404907975460138E-2</v>
       </c>
-      <c r="J18" s="1">
-        <f t="shared" si="1"/>
+      <c r="L18" s="1">
+        <f t="shared" si="3"/>
         <v>0.19736842105263158</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
@@ -1741,17 +1887,25 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" si="0"/>
+        <v>-4.9999999999999489E-3</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.124</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="2"/>
         <v>-1.4492753623188259E-2</v>
       </c>
-      <c r="J19" s="8">
-        <f t="shared" si="1"/>
+      <c r="L19" s="1">
+        <f t="shared" si="3"/>
         <v>-5.6363636363636367</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1778,17 +1932,25 @@
       </c>
       <c r="I20" s="1">
         <f t="shared" si="0"/>
+        <v>-6.0000000000000053E-3</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1999999999999983E-2</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="2"/>
         <v>-2.3255813953488393E-2</v>
       </c>
-      <c r="J20" s="1">
-        <f t="shared" si="1"/>
+      <c r="L20" s="1">
+        <f t="shared" si="3"/>
         <v>7.1428571428571327E-2</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
@@ -1815,17 +1977,25 @@
       </c>
       <c r="I21" s="1">
         <f t="shared" si="0"/>
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0000000000000036E-3</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="2"/>
         <v>-0.1931818181818182</v>
       </c>
-      <c r="J21" s="1">
-        <f t="shared" si="1"/>
+      <c r="L21" s="1">
+        <f t="shared" si="3"/>
         <v>5.1948051948051993E-2</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1852,17 +2022,25 @@
       </c>
       <c r="I22" s="1">
         <f t="shared" si="0"/>
+        <v>-0.47699999999999998</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.161</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="2"/>
         <v>-8.3684210526315788</v>
       </c>
-      <c r="J22" s="8">
-        <f t="shared" si="1"/>
+      <c r="L22" s="1">
+        <f t="shared" si="3"/>
         <v>-4.2368421052631584</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1889,17 +2067,25 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
+        <v>-0.83100000000000007</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.0640000000000001</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="2"/>
         <v>-0.8935483870967742</v>
       </c>
-      <c r="J23" s="8">
-        <f t="shared" si="1"/>
+      <c r="L23" s="1">
+        <f t="shared" si="3"/>
         <v>-1.0534653465346535</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1926,17 +2112,25 @@
       </c>
       <c r="I24" s="1">
         <f t="shared" si="0"/>
+        <v>-2.1020000000000003</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.70399999999999996</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="2"/>
         <v>-1.3055900621118013</v>
       </c>
-      <c r="J24" s="8">
-        <f t="shared" si="1"/>
+      <c r="L24" s="1">
+        <f t="shared" si="3"/>
         <v>-2.5053380782918144</v>
       </c>
-      <c r="K24" t="s">
+      <c r="M24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
@@ -1963,17 +2157,25 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" si="0"/>
+        <v>-0.16999999999999998</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="1"/>
+        <v>-2.0000000000000018E-3</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="2"/>
         <v>-0.83333333333333326</v>
       </c>
-      <c r="J25" s="1">
-        <f t="shared" si="1"/>
+      <c r="L25" s="1">
+        <f t="shared" si="3"/>
         <v>-1.4598540145985413E-2</v>
       </c>
-      <c r="K25" t="s">
+      <c r="M25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -2000,17 +2202,25 @@
       </c>
       <c r="I26" s="1">
         <f t="shared" si="0"/>
+        <v>-6.2E-2</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="1"/>
+        <v>-1.8000000000000002E-2</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="2"/>
         <v>-0.29523809523809524</v>
       </c>
-      <c r="J26" s="1">
-        <f t="shared" si="1"/>
+      <c r="L26" s="1">
+        <f t="shared" si="3"/>
         <v>-0.1475409836065574</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -2037,17 +2247,25 @@
       </c>
       <c r="I27" s="1">
         <f t="shared" si="0"/>
+        <v>-0.22000000000000003</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.218</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="2"/>
         <v>-0.82397003745318353</v>
       </c>
-      <c r="J27" s="8">
-        <f t="shared" si="1"/>
+      <c r="L27" s="1">
+        <f t="shared" si="3"/>
         <v>-1.231638418079096</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -2072,19 +2290,27 @@
       <c r="H28">
         <v>-4.9000000000000002E-2</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.48400000000000004</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="1"/>
+        <v>-6.3E-2</v>
+      </c>
+      <c r="K28" s="1">
         <f>(F28-E28)/ABS(E28)</f>
         <v>-11.000000000000002</v>
       </c>
-      <c r="J28" s="8">
-        <f t="shared" si="1"/>
+      <c r="L28" s="1">
+        <f t="shared" si="3"/>
         <v>-4.5</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
@@ -2109,19 +2335,27 @@
       <c r="H29">
         <v>-6.2E-2</v>
       </c>
-      <c r="I29" s="9">
-        <f t="shared" si="0"/>
+      <c r="I29" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.69500000000000006</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.158</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="2"/>
         <v>-28.958333333333336</v>
       </c>
-      <c r="J29" s="8">
-        <f t="shared" si="1"/>
+      <c r="L29" s="1">
+        <f t="shared" si="3"/>
         <v>-1.6458333333333333</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
@@ -2148,23 +2382,31 @@
       </c>
       <c r="I30" s="1">
         <f t="shared" si="0"/>
+        <v>-0.14800000000000002</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="1"/>
+        <v>-6.2E-2</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="2"/>
         <v>-0.88622754491017974</v>
       </c>
-      <c r="J30" s="1">
-        <f t="shared" si="1"/>
+      <c r="L30" s="1">
+        <f t="shared" si="3"/>
         <v>-0.5535714285714286</v>
       </c>
-      <c r="K30" t="s">
+      <c r="M30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="I28" formula="1"/>
+    <ignoredError sqref="K28" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ran updated DDE model with diurnal variation
</commit_message>
<xml_diff>
--- a/Model results Tmax.xlsx
+++ b/Model results Tmax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24D8B7F-24BD-544F-A78B-17F0E1C179A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9053FB5-61AF-F149-9ED1-C3FF23CD894A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="24120" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="27440" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="58">
   <si>
     <t>Species</t>
   </si>
@@ -189,6 +189,21 @@
   </si>
   <si>
     <t>delta.prop.model</t>
+  </si>
+  <si>
+    <t>rMax</t>
+  </si>
+  <si>
+    <t>TPC historical</t>
+  </si>
+  <si>
+    <t>TPC future</t>
+  </si>
+  <si>
+    <t>Model historical</t>
+  </si>
+  <si>
+    <t>Model future</t>
   </si>
 </sst>
 </file>
@@ -346,7 +361,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,8 +541,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -642,6 +663,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -687,7 +757,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -696,7 +766,18 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1052,61 +1133,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="K1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1119,39 +1220,58 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="F2" s="9">
         <v>0.105</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="6">
         <v>3.1E-2</v>
       </c>
-      <c r="G2" s="5">
+      <c r="H2" s="5">
         <v>7.8E-2</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <v>-2E-3</v>
       </c>
-      <c r="I2" s="1">
-        <f>F2-E2</f>
-        <v>-7.3999999999999996E-2</v>
-      </c>
-      <c r="J2" s="1">
-        <f>H2-G2</f>
-        <v>-0.08</v>
-      </c>
-      <c r="K2" s="1">
-        <f>(F2-E2)/E2</f>
+      <c r="J2" s="10">
+        <f>F2/$E2</f>
+        <v>0.78358208955223874</v>
+      </c>
+      <c r="K2" s="16">
+        <f>G2/$E2</f>
+        <v>0.23134328358208953</v>
+      </c>
+      <c r="L2" s="16">
+        <f>H2/$E2</f>
+        <v>0.58208955223880599</v>
+      </c>
+      <c r="M2" s="18">
+        <f>I2/$E2</f>
+        <v>-1.4925373134328358E-2</v>
+      </c>
+      <c r="N2" s="1">
+        <f>K2-J2</f>
+        <v>-0.55223880597014918</v>
+      </c>
+      <c r="O2" s="1">
+        <f>M2-L2</f>
+        <v>-0.59701492537313439</v>
+      </c>
+      <c r="P2" s="11">
+        <f>(K2-J2)/J2</f>
         <v>-0.7047619047619047</v>
       </c>
-      <c r="L2" s="1">
-        <f>(H2-G2)/G2</f>
+      <c r="Q2" s="1">
+        <f>(M2-L2)/L2</f>
         <v>-1.0256410256410258</v>
       </c>
-      <c r="M2" t="s">
+      <c r="R2" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1164,36 +1284,56 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3">
+        <v>0.154</v>
+      </c>
+      <c r="F3" s="10">
         <v>0.14899999999999999</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>0.14499999999999999</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="5">
         <v>0.114</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>0.14099999999999999</v>
       </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I30" si="0">F3-E3</f>
-        <v>-4.0000000000000036E-3</v>
-      </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J30" si="1">H3-G3</f>
-        <v>2.6999999999999982E-2</v>
-      </c>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3:K30" si="2">(F3-E3)/E3</f>
-        <v>-2.6845637583892641E-2</v>
-      </c>
-      <c r="L3" s="1">
-        <f t="shared" ref="L3:L30" si="3">(H3-G3)/G3</f>
+      <c r="J3" s="10">
+        <f t="shared" ref="J3:J30" si="0">F3/$E3</f>
+        <v>0.96753246753246747</v>
+      </c>
+      <c r="K3" s="16">
+        <f t="shared" ref="K3:K30" si="1">G3/$E3</f>
+        <v>0.94155844155844148</v>
+      </c>
+      <c r="L3" s="16">
+        <f t="shared" ref="L3:L30" si="2">H3/$E3</f>
+        <v>0.74025974025974028</v>
+      </c>
+      <c r="M3" s="18">
+        <f t="shared" ref="M3:M30" si="3">I3/$E3</f>
+        <v>0.9155844155844155</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" ref="N3:N30" si="4">K3-J3</f>
+        <v>-2.5974025974025983E-2</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" ref="O3:O30" si="5">M3-L3</f>
+        <v>0.17532467532467522</v>
+      </c>
+      <c r="P3" s="11">
+        <f t="shared" ref="P3:P30" si="6">(K3-J3)/J3</f>
+        <v>-2.6845637583892627E-2</v>
+      </c>
+      <c r="Q3" s="1">
+        <f t="shared" ref="Q3:Q30" si="7">(M3-L3)/L3</f>
         <v>0.23684210526315774</v>
       </c>
+      <c r="R3" s="8"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1206,36 +1346,56 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4">
+        <v>0.154</v>
+      </c>
+      <c r="F4" s="10">
         <v>0.14599999999999999</v>
       </c>
-      <c r="F4" s="6">
+      <c r="G4" s="6">
         <v>0.104</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <v>0.13600000000000001</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="10">
         <f t="shared" si="0"/>
-        <v>-4.1999999999999996E-2</v>
-      </c>
-      <c r="J4" s="1">
+        <v>0.94805194805194803</v>
+      </c>
+      <c r="K4" s="16">
         <f t="shared" si="1"/>
-        <v>-9.5000000000000001E-2</v>
-      </c>
-      <c r="K4" s="1">
+        <v>0.67532467532467533</v>
+      </c>
+      <c r="L4" s="16">
         <f t="shared" si="2"/>
+        <v>0.88311688311688319</v>
+      </c>
+      <c r="M4" s="18">
+        <f t="shared" si="3"/>
+        <v>0.26623376623376627</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.27272727272727271</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.61688311688311692</v>
+      </c>
+      <c r="P4" s="11">
+        <f t="shared" si="6"/>
         <v>-0.28767123287671231</v>
       </c>
-      <c r="L4" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q4" s="1">
+        <f t="shared" si="7"/>
         <v>-0.69852941176470584</v>
       </c>
+      <c r="R4" s="8"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1248,39 +1408,58 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
+        <v>0.104</v>
+      </c>
+      <c r="F5" s="9">
         <v>0.10100000000000001</v>
       </c>
-      <c r="F5" s="6">
+      <c r="G5" s="6">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <v>0.17199999999999999</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>-4.2999999999999997E-2</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="10">
         <f t="shared" si="0"/>
-        <v>-1.9000000000000003E-2</v>
-      </c>
-      <c r="J5" s="1">
+        <v>0.97115384615384626</v>
+      </c>
+      <c r="K5" s="16">
         <f t="shared" si="1"/>
-        <v>-0.21499999999999997</v>
-      </c>
-      <c r="K5" s="1">
+        <v>0.78846153846153855</v>
+      </c>
+      <c r="L5" s="19">
         <f t="shared" si="2"/>
-        <v>-0.18811881188118815</v>
-      </c>
-      <c r="L5" s="1">
+        <v>1.6538461538461537</v>
+      </c>
+      <c r="M5" s="18">
         <f t="shared" si="3"/>
+        <v>-0.41346153846153844</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.18269230769230771</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="5"/>
+        <v>-2.0673076923076921</v>
+      </c>
+      <c r="P5" s="11">
+        <f t="shared" si="6"/>
+        <v>-0.18811881188118812</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="7"/>
         <v>-1.25</v>
       </c>
-      <c r="M5" t="s">
+      <c r="R5" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1293,39 +1472,58 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="F6" s="10">
         <v>0.113</v>
       </c>
-      <c r="F6" s="6">
+      <c r="G6" s="6">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="10">
         <f t="shared" si="0"/>
-        <v>-0.183</v>
-      </c>
-      <c r="J6" s="1">
+        <v>0.68484848484848482</v>
+      </c>
+      <c r="K6" s="16">
         <f t="shared" si="1"/>
-        <v>-4.0000000000000008E-2</v>
-      </c>
-      <c r="K6" s="1">
+        <v>-0.42424242424242425</v>
+      </c>
+      <c r="L6" s="16">
         <f t="shared" si="2"/>
-        <v>-1.6194690265486724</v>
-      </c>
-      <c r="L6" s="1">
+        <v>0.41818181818181821</v>
+      </c>
+      <c r="M6" s="18">
         <f t="shared" si="3"/>
+        <v>0.17575757575757575</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.1090909090909091</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.24242424242424246</v>
+      </c>
+      <c r="P6" s="11">
+        <f t="shared" si="6"/>
+        <v>-1.6194690265486726</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="7"/>
         <v>-0.57971014492753625</v>
       </c>
-      <c r="M6" t="s">
+      <c r="R6" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1338,39 +1536,58 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F7" s="10">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="F7" s="6">
+      <c r="G7" s="6">
         <v>0.05</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="5">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="6">
         <v>0.03</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="10">
         <f t="shared" si="0"/>
-        <v>-9.9999999999999395E-4</v>
-      </c>
-      <c r="J7" s="1">
+        <v>0.61445783132530118</v>
+      </c>
+      <c r="K7" s="16">
         <f t="shared" si="1"/>
-        <v>-2.8999999999999998E-2</v>
-      </c>
-      <c r="K7" s="1">
+        <v>0.60240963855421692</v>
+      </c>
+      <c r="L7" s="16">
         <f t="shared" si="2"/>
+        <v>0.71084337349397586</v>
+      </c>
+      <c r="M7" s="18">
+        <f t="shared" si="3"/>
+        <v>0.36144578313253006</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.2048192771084265E-2</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.3493975903614458</v>
+      </c>
+      <c r="P7" s="11">
+        <f t="shared" si="6"/>
         <v>-1.9607843137254784E-2</v>
       </c>
-      <c r="L7" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.49152542372881353</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="Q7" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.49152542372881358</v>
+      </c>
+      <c r="R7" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1383,39 +1600,58 @@
       <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="F8" s="9">
         <v>0.11899999999999999</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G8" s="6">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="10">
         <f t="shared" si="0"/>
-        <v>-7.3999999999999996E-2</v>
-      </c>
-      <c r="J8" s="1">
+        <v>0.72121212121212119</v>
+      </c>
+      <c r="K8" s="16">
         <f t="shared" si="1"/>
-        <v>-2.0999999999999998E-2</v>
-      </c>
-      <c r="K8" s="1">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="L8" s="16">
         <f t="shared" si="2"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="M8" s="18">
+        <f t="shared" si="3"/>
+        <v>0.32727272727272727</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.44848484848484849</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.12727272727272726</v>
+      </c>
+      <c r="P8" s="11">
+        <f t="shared" si="6"/>
         <v>-0.62184873949579833</v>
       </c>
-      <c r="L8" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q8" s="1">
+        <f t="shared" si="7"/>
         <v>-0.27999999999999997</v>
       </c>
-      <c r="M8" t="s">
+      <c r="R8" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1428,39 +1664,58 @@
       <c r="D9" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F9" s="10">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="F9" s="6">
+      <c r="G9" s="6">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="10">
         <f t="shared" si="0"/>
-        <v>-1.1000000000000003E-2</v>
-      </c>
-      <c r="J9" s="1">
+        <v>0.6506024096385542</v>
+      </c>
+      <c r="K9" s="16">
         <f t="shared" si="1"/>
-        <v>-2.9000000000000001E-2</v>
-      </c>
-      <c r="K9" s="1">
+        <v>0.5180722891566264</v>
+      </c>
+      <c r="L9" s="16">
         <f t="shared" si="2"/>
-        <v>-0.20370370370370375</v>
-      </c>
-      <c r="L9" s="1">
+        <v>0.68674698795180722</v>
+      </c>
+      <c r="M9" s="18">
         <f t="shared" si="3"/>
+        <v>0.33734939759036142</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.1325301204819278</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.3493975903614458</v>
+      </c>
+      <c r="P9" s="11">
+        <f t="shared" si="6"/>
+        <v>-0.20370370370370386</v>
+      </c>
+      <c r="Q9" s="1">
+        <f t="shared" si="7"/>
         <v>-0.50877192982456143</v>
       </c>
-      <c r="M9" t="s">
+      <c r="R9" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1473,36 +1728,56 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10">
+        <v>0.246</v>
+      </c>
+      <c r="F10" s="10">
         <v>0.186</v>
       </c>
-      <c r="F10" s="6">
+      <c r="G10" s="6">
         <v>0.12</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="5">
         <v>0.38100000000000001</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>0.14599999999999999</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="10">
         <f t="shared" si="0"/>
-        <v>-6.6000000000000003E-2</v>
-      </c>
-      <c r="J10" s="1">
+        <v>0.75609756097560976</v>
+      </c>
+      <c r="K10" s="16">
         <f t="shared" si="1"/>
-        <v>-0.23500000000000001</v>
-      </c>
-      <c r="K10" s="1">
+        <v>0.48780487804878048</v>
+      </c>
+      <c r="L10" s="19">
         <f t="shared" si="2"/>
+        <v>1.5487804878048781</v>
+      </c>
+      <c r="M10" s="18">
+        <f t="shared" si="3"/>
+        <v>0.5934959349593496</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.26829268292682928</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.95528455284552849</v>
+      </c>
+      <c r="P10" s="11">
+        <f t="shared" si="6"/>
         <v>-0.35483870967741937</v>
       </c>
-      <c r="L10" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q10" s="1">
+        <f t="shared" si="7"/>
         <v>-0.61679790026246717</v>
       </c>
+      <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1515,40 +1790,59 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="F11" s="10">
         <v>0.13800000000000001</v>
       </c>
-      <c r="F11" s="6">
+      <c r="G11" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <v>0.19400000000000001</v>
       </c>
-      <c r="H11" s="7">
+      <c r="I11" s="7">
         <f>-1.62</f>
         <v>-1.62</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="10">
         <f t="shared" si="0"/>
-        <v>-0.13</v>
-      </c>
-      <c r="J11" s="1">
+        <v>0.53696498054474706</v>
+      </c>
+      <c r="K11" s="16">
         <f t="shared" si="1"/>
-        <v>-1.8140000000000001</v>
-      </c>
-      <c r="K11" s="1">
+        <v>3.1128404669260701E-2</v>
+      </c>
+      <c r="L11" s="16">
         <f t="shared" si="2"/>
+        <v>0.75486381322957197</v>
+      </c>
+      <c r="M11" s="18">
+        <f t="shared" si="3"/>
+        <v>-6.3035019455252925</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.50583657587548636</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="5"/>
+        <v>-7.0583657587548645</v>
+      </c>
+      <c r="P11" s="11">
+        <f t="shared" si="6"/>
         <v>-0.94202898550724634</v>
       </c>
-      <c r="L11" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q11" s="1">
+        <f t="shared" si="7"/>
         <v>-9.3505154639175263</v>
       </c>
-      <c r="M11" t="s">
+      <c r="R11" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1561,36 +1855,56 @@
       <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12">
+        <v>0.249</v>
+      </c>
+      <c r="F12" s="9">
         <v>0.14299999999999999</v>
       </c>
-      <c r="F12" s="6">
+      <c r="G12" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="6">
         <v>0.53</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>0.159</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="10">
         <f t="shared" si="0"/>
-        <v>-0.13599999999999998</v>
-      </c>
-      <c r="J12" s="1">
+        <v>0.57429718875502</v>
+      </c>
+      <c r="K12" s="16">
         <f t="shared" si="1"/>
-        <v>-0.371</v>
-      </c>
-      <c r="K12" s="1">
+        <v>2.8112449799196786E-2</v>
+      </c>
+      <c r="L12" s="19">
         <f t="shared" si="2"/>
+        <v>2.1285140562248999</v>
+      </c>
+      <c r="M12" s="18">
+        <f t="shared" si="3"/>
+        <v>0.63855421686746994</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.5461847389558232</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="5"/>
+        <v>-1.48995983935743</v>
+      </c>
+      <c r="P12" s="11">
+        <f t="shared" si="6"/>
         <v>-0.95104895104895104</v>
       </c>
-      <c r="L12" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.7</v>
-      </c>
+      <c r="Q12" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.70000000000000007</v>
+      </c>
+      <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1604,38 +1918,57 @@
         <v>11</v>
       </c>
       <c r="E13" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="11">
         <v>0.06</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="4">
         <v>-1.7999999999999999E-2</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="10">
         <f t="shared" si="0"/>
-        <v>-8.5999999999999993E-2</v>
-      </c>
-      <c r="J13" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K13" s="16">
         <f t="shared" si="1"/>
-        <v>-8.5000000000000006E-2</v>
-      </c>
-      <c r="K13" s="1">
+        <v>-0.25999999999999995</v>
+      </c>
+      <c r="L13" s="16">
         <f t="shared" si="2"/>
-        <v>-1.4333333333333333</v>
-      </c>
-      <c r="L13" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="M13" s="18">
         <f t="shared" si="3"/>
-        <v>-1.2686567164179106</v>
-      </c>
-      <c r="M13" t="s">
+        <v>-0.17999999999999997</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.85999999999999988</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.85</v>
+      </c>
+      <c r="P13" s="11">
+        <f t="shared" si="6"/>
+        <v>-1.4333333333333331</v>
+      </c>
+      <c r="Q13" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.2686567164179103</v>
+      </c>
+      <c r="R13" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1648,39 +1981,58 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
+        <v>0.104</v>
+      </c>
+      <c r="F14" s="11">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>-0.125</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="4">
         <v>-2.1999999999999999E-2</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="10">
         <f t="shared" si="0"/>
-        <v>-0.17699999999999999</v>
-      </c>
-      <c r="J14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="16">
         <f t="shared" si="1"/>
-        <v>-9.4E-2</v>
-      </c>
-      <c r="K14" s="1">
+        <v>-1.2019230769230769</v>
+      </c>
+      <c r="L14" s="16">
         <f t="shared" si="2"/>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="M14" s="18">
+        <f t="shared" si="3"/>
+        <v>-0.21153846153846154</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.7019230769230769</v>
+      </c>
+      <c r="O14" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.90384615384615385</v>
+      </c>
+      <c r="P14" s="11">
+        <f t="shared" si="6"/>
         <v>-3.4038461538461537</v>
       </c>
-      <c r="L14" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q14" s="1">
+        <f t="shared" si="7"/>
         <v>-1.3055555555555556</v>
       </c>
-      <c r="M14" t="s">
+      <c r="R14" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1693,39 +2045,58 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="F15" s="11">
         <v>0.23400000000000001</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>0.11</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>7.8E-2</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>-5.5E-2</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="10">
         <f t="shared" si="0"/>
-        <v>-0.12400000000000001</v>
-      </c>
-      <c r="J15" s="1">
+        <v>0.48347107438016534</v>
+      </c>
+      <c r="K15" s="16">
         <f t="shared" si="1"/>
-        <v>-0.13300000000000001</v>
-      </c>
-      <c r="K15" s="1">
+        <v>0.22727272727272729</v>
+      </c>
+      <c r="L15" s="16">
         <f t="shared" si="2"/>
+        <v>0.16115702479338845</v>
+      </c>
+      <c r="M15" s="18">
+        <f t="shared" si="3"/>
+        <v>-0.11363636363636365</v>
+      </c>
+      <c r="N15" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.25619834710743805</v>
+      </c>
+      <c r="O15" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.27479338842975209</v>
+      </c>
+      <c r="P15" s="11">
+        <f t="shared" si="6"/>
         <v>-0.52991452991452992</v>
       </c>
-      <c r="L15" s="1">
-        <f t="shared" si="3"/>
-        <v>-1.7051282051282053</v>
-      </c>
-      <c r="M15" t="s">
+      <c r="Q15" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.7051282051282051</v>
+      </c>
+      <c r="R15" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1738,39 +2109,58 @@
       <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16">
+        <v>0.436</v>
+      </c>
+      <c r="F16" s="11">
         <v>0.253</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>0.16200000000000001</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="10">
         <f t="shared" si="0"/>
-        <v>-9.0999999999999998E-2</v>
-      </c>
-      <c r="J16" s="1">
+        <v>0.58027522935779818</v>
+      </c>
+      <c r="K16" s="16">
         <f t="shared" si="1"/>
-        <v>-1.4999999999999993E-2</v>
-      </c>
-      <c r="K16" s="1">
+        <v>0.37155963302752293</v>
+      </c>
+      <c r="L16" s="16">
         <f t="shared" si="2"/>
-        <v>-0.35968379446640314</v>
-      </c>
-      <c r="L16" s="1">
+        <v>0.1628440366972477</v>
+      </c>
+      <c r="M16" s="18">
         <f t="shared" si="3"/>
-        <v>-0.21126760563380273</v>
-      </c>
-      <c r="M16" t="s">
+        <v>0.12844036697247707</v>
+      </c>
+      <c r="N16" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.20871559633027525</v>
+      </c>
+      <c r="O16" s="1">
+        <f t="shared" si="5"/>
+        <v>-3.440366972477063E-2</v>
+      </c>
+      <c r="P16" s="11">
+        <f t="shared" si="6"/>
+        <v>-0.35968379446640319</v>
+      </c>
+      <c r="Q16" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.21126760563380276</v>
+      </c>
+      <c r="R16" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
@@ -1783,39 +2173,58 @@
       <c r="D17" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F17" s="11">
         <v>0.16700000000000001</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>0.19500000000000001</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>0.106</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="10">
         <f t="shared" si="0"/>
-        <v>2.7999999999999997E-2</v>
-      </c>
-      <c r="J17" s="1">
+        <v>0.58391608391608396</v>
+      </c>
+      <c r="K17" s="16">
         <f t="shared" si="1"/>
-        <v>-1.8000000000000002E-2</v>
-      </c>
-      <c r="K17" s="1">
+        <v>0.68181818181818188</v>
+      </c>
+      <c r="L17" s="16">
         <f t="shared" si="2"/>
-        <v>0.1676646706586826</v>
-      </c>
-      <c r="L17" s="1">
+        <v>0.37062937062937062</v>
+      </c>
+      <c r="M17" s="18">
         <f t="shared" si="3"/>
-        <v>-0.169811320754717</v>
-      </c>
-      <c r="M17" t="s">
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="N17" s="1">
+        <f t="shared" si="4"/>
+        <v>9.7902097902097918E-2</v>
+      </c>
+      <c r="O17" s="1">
+        <f t="shared" si="5"/>
+        <v>-6.2937062937062915E-2</v>
+      </c>
+      <c r="P17" s="11">
+        <f t="shared" si="6"/>
+        <v>0.16766467065868265</v>
+      </c>
+      <c r="Q17" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.16981132075471692</v>
+      </c>
+      <c r="R17" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -1828,39 +2237,58 @@
       <c r="D18" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="F18" s="11">
         <v>0.16300000000000001</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>0.16600000000000001</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="10">
         <f t="shared" si="0"/>
-        <v>3.0000000000000027E-3</v>
-      </c>
-      <c r="J18" s="1">
+        <v>0.84020618556701032</v>
+      </c>
+      <c r="K18" s="16">
         <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="K18" s="1">
+        <v>0.85567010309278357</v>
+      </c>
+      <c r="L18" s="16">
         <f t="shared" si="2"/>
-        <v>1.8404907975460138E-2</v>
-      </c>
-      <c r="L18" s="1">
+        <v>0.39175257731958762</v>
+      </c>
+      <c r="M18" s="18">
         <f t="shared" si="3"/>
+        <v>0.46907216494845361</v>
+      </c>
+      <c r="N18" s="1">
+        <f t="shared" si="4"/>
+        <v>1.5463917525773252E-2</v>
+      </c>
+      <c r="O18" s="1">
+        <f t="shared" si="5"/>
+        <v>7.7319587628865982E-2</v>
+      </c>
+      <c r="P18" s="11">
+        <f t="shared" si="6"/>
+        <v>1.840490797546019E-2</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" si="7"/>
         <v>0.19736842105263158</v>
       </c>
-      <c r="M18" t="s">
+      <c r="R18" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
@@ -1873,39 +2301,58 @@
       <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19">
+        <v>0.443</v>
+      </c>
+      <c r="F19" s="11">
         <v>0.34499999999999997</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>0.34</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="H19" s="4">
+      <c r="I19" s="4">
         <v>-0.10199999999999999</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="10">
         <f t="shared" si="0"/>
-        <v>-4.9999999999999489E-3</v>
-      </c>
-      <c r="J19" s="1">
+        <v>0.77878103837471779</v>
+      </c>
+      <c r="K19" s="16">
         <f t="shared" si="1"/>
-        <v>-0.124</v>
-      </c>
-      <c r="K19" s="1">
+        <v>0.76749435665914223</v>
+      </c>
+      <c r="L19" s="16">
         <f t="shared" si="2"/>
-        <v>-1.4492753623188259E-2</v>
-      </c>
-      <c r="L19" s="1">
+        <v>4.9661399548532728E-2</v>
+      </c>
+      <c r="M19" s="18">
         <f t="shared" si="3"/>
+        <v>-0.23024830699774265</v>
+      </c>
+      <c r="N19" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.1286681715575564E-2</v>
+      </c>
+      <c r="O19" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.27990970654627539</v>
+      </c>
+      <c r="P19" s="11">
+        <f t="shared" si="6"/>
+        <v>-1.4492753623188333E-2</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="7"/>
         <v>-5.6363636363636367</v>
       </c>
-      <c r="M19" t="s">
+      <c r="R19" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1918,39 +2365,58 @@
       <c r="D20" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="F20" s="11">
         <v>0.25800000000000001</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>0.252</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>0.16800000000000001</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>0.18</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="10">
         <f t="shared" si="0"/>
-        <v>-6.0000000000000053E-3</v>
-      </c>
-      <c r="J20" s="1">
+        <v>0.84313725490196079</v>
+      </c>
+      <c r="K20" s="16">
         <f t="shared" si="1"/>
-        <v>1.1999999999999983E-2</v>
-      </c>
-      <c r="K20" s="1">
+        <v>0.82352941176470595</v>
+      </c>
+      <c r="L20" s="16">
         <f t="shared" si="2"/>
-        <v>-2.3255813953488393E-2</v>
-      </c>
-      <c r="L20" s="1">
+        <v>0.5490196078431373</v>
+      </c>
+      <c r="M20" s="18">
         <f t="shared" si="3"/>
-        <v>7.1428571428571327E-2</v>
-      </c>
-      <c r="M20" t="s">
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="N20" s="1">
+        <f t="shared" si="4"/>
+        <v>-1.9607843137254832E-2</v>
+      </c>
+      <c r="O20" s="1">
+        <f t="shared" si="5"/>
+        <v>3.9215686274509776E-2</v>
+      </c>
+      <c r="P20" s="11">
+        <f t="shared" si="6"/>
+        <v>-2.3255813953488289E-2</v>
+      </c>
+      <c r="Q20" s="1">
+        <f t="shared" si="7"/>
+        <v>7.1428571428571369E-2</v>
+      </c>
+      <c r="R20" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
@@ -1963,39 +2429,58 @@
       <c r="D21" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="F21" s="11">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="10">
         <f t="shared" si="0"/>
-        <v>-1.7000000000000001E-2</v>
-      </c>
-      <c r="J21" s="1">
+        <v>0.44221105527638188</v>
+      </c>
+      <c r="K21" s="16">
         <f t="shared" si="1"/>
-        <v>4.0000000000000036E-3</v>
-      </c>
-      <c r="K21" s="1">
+        <v>0.35678391959798988</v>
+      </c>
+      <c r="L21" s="16">
         <f t="shared" si="2"/>
-        <v>-0.1931818181818182</v>
-      </c>
-      <c r="L21" s="1">
+        <v>0.38693467336683413</v>
+      </c>
+      <c r="M21" s="18">
         <f t="shared" si="3"/>
-        <v>5.1948051948051993E-2</v>
-      </c>
-      <c r="M21" t="s">
+        <v>0.40703517587939697</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" si="4"/>
+        <v>-8.5427135678391997E-2</v>
+      </c>
+      <c r="O21" s="1">
+        <f t="shared" si="5"/>
+        <v>2.0100502512562846E-2</v>
+      </c>
+      <c r="P21" s="11">
+        <f t="shared" si="6"/>
+        <v>-0.19318181818181829</v>
+      </c>
+      <c r="Q21" s="1">
+        <f t="shared" si="7"/>
+        <v>5.1948051948052035E-2</v>
+      </c>
+      <c r="R21" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
@@ -2008,39 +2493,58 @@
       <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="F22" s="11">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>-0.42</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>-0.123</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="10">
         <f t="shared" si="0"/>
-        <v>-0.47699999999999998</v>
-      </c>
-      <c r="J22" s="1">
+        <v>0.27941176470588236</v>
+      </c>
+      <c r="K22" s="16">
         <f t="shared" si="1"/>
-        <v>-0.161</v>
-      </c>
-      <c r="K22" s="1">
+        <v>-2.0588235294117649</v>
+      </c>
+      <c r="L22" s="16">
         <f t="shared" si="2"/>
+        <v>0.18627450980392157</v>
+      </c>
+      <c r="M22" s="18">
+        <f t="shared" si="3"/>
+        <v>-0.60294117647058831</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.3382352941176472</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.78921568627450989</v>
+      </c>
+      <c r="P22" s="11">
+        <f t="shared" si="6"/>
         <v>-8.3684210526315788</v>
       </c>
-      <c r="L22" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q22" s="1">
+        <f t="shared" si="7"/>
         <v>-4.2368421052631584</v>
       </c>
-      <c r="M22" t="s">
+      <c r="R22" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2053,39 +2557,58 @@
       <c r="D23" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
+        <v>1.49</v>
+      </c>
+      <c r="F23" s="12">
         <v>0.93</v>
       </c>
-      <c r="F23" s="3">
+      <c r="G23" s="3">
         <v>9.9000000000000005E-2</v>
       </c>
-      <c r="G23" s="3">
+      <c r="H23" s="3">
         <v>1.01</v>
       </c>
-      <c r="H23" s="4">
+      <c r="I23" s="4">
         <v>-5.3999999999999999E-2</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="10">
         <f t="shared" si="0"/>
-        <v>-0.83100000000000007</v>
-      </c>
-      <c r="J23" s="1">
+        <v>0.62416107382550334</v>
+      </c>
+      <c r="K23" s="16">
         <f t="shared" si="1"/>
-        <v>-1.0640000000000001</v>
-      </c>
-      <c r="K23" s="1">
+        <v>6.6442953020134227E-2</v>
+      </c>
+      <c r="L23" s="16">
         <f t="shared" si="2"/>
+        <v>0.67785234899328861</v>
+      </c>
+      <c r="M23" s="18">
+        <f t="shared" si="3"/>
+        <v>-3.6241610738255034E-2</v>
+      </c>
+      <c r="N23" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.55771812080536909</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.71409395973154366</v>
+      </c>
+      <c r="P23" s="11">
+        <f t="shared" si="6"/>
         <v>-0.8935483870967742</v>
       </c>
-      <c r="L23" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q23" s="1">
+        <f t="shared" si="7"/>
         <v>-1.0534653465346535</v>
       </c>
-      <c r="M23" t="s">
+      <c r="R23" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -2098,39 +2621,58 @@
       <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24">
+        <v>3.42</v>
+      </c>
+      <c r="F24" s="13">
         <v>1.61</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>-0.49199999999999999</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>0.28100000000000003</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>-0.42299999999999999</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="10">
         <f t="shared" si="0"/>
-        <v>-2.1020000000000003</v>
-      </c>
-      <c r="J24" s="1">
+        <v>0.47076023391812871</v>
+      </c>
+      <c r="K24" s="16">
         <f t="shared" si="1"/>
-        <v>-0.70399999999999996</v>
-      </c>
-      <c r="K24" s="1">
+        <v>-0.14385964912280702</v>
+      </c>
+      <c r="L24" s="16">
         <f t="shared" si="2"/>
+        <v>8.2163742690058494E-2</v>
+      </c>
+      <c r="M24" s="18">
+        <f t="shared" si="3"/>
+        <v>-0.12368421052631579</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.61461988304093573</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.20584795321637428</v>
+      </c>
+      <c r="P24" s="11">
+        <f t="shared" si="6"/>
         <v>-1.3055900621118013</v>
       </c>
-      <c r="L24" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q24" s="1">
+        <f t="shared" si="7"/>
         <v>-2.5053380782918144</v>
       </c>
-      <c r="M24" t="s">
+      <c r="R24" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
@@ -2143,39 +2685,58 @@
       <c r="D25" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="F25" s="11">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>0.13700000000000001</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>0.13500000000000001</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="10">
         <f t="shared" si="0"/>
-        <v>-0.16999999999999998</v>
-      </c>
-      <c r="J25" s="1">
+        <v>0.61445783132530118</v>
+      </c>
+      <c r="K25" s="16">
         <f t="shared" si="1"/>
-        <v>-2.0000000000000018E-3</v>
-      </c>
-      <c r="K25" s="1">
+        <v>0.10240963855421686</v>
+      </c>
+      <c r="L25" s="16">
         <f t="shared" si="2"/>
+        <v>0.41265060240963858</v>
+      </c>
+      <c r="M25" s="18">
+        <f t="shared" si="3"/>
+        <v>0.40662650602409639</v>
+      </c>
+      <c r="N25" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.51204819277108427</v>
+      </c>
+      <c r="O25" s="1">
+        <f t="shared" si="5"/>
+        <v>-6.0240963855421881E-3</v>
+      </c>
+      <c r="P25" s="11">
+        <f t="shared" si="6"/>
         <v>-0.83333333333333326</v>
       </c>
-      <c r="L25" s="1">
-        <f t="shared" si="3"/>
-        <v>-1.4598540145985413E-2</v>
-      </c>
-      <c r="M25" t="s">
+      <c r="Q25" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.4598540145985448E-2</v>
+      </c>
+      <c r="R25" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -2188,39 +2749,58 @@
       <c r="D26" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="F26" s="11">
         <v>0.21</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>0.14799999999999999</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>0.122</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>0.104</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="10">
         <f t="shared" si="0"/>
-        <v>-6.2E-2</v>
-      </c>
-      <c r="J26" s="1">
+        <v>0.52896725440806036</v>
+      </c>
+      <c r="K26" s="16">
         <f t="shared" si="1"/>
-        <v>-1.8000000000000002E-2</v>
-      </c>
-      <c r="K26" s="1">
+        <v>0.37279596977329971</v>
+      </c>
+      <c r="L26" s="16">
         <f t="shared" si="2"/>
-        <v>-0.29523809523809524</v>
-      </c>
-      <c r="L26" s="1">
+        <v>0.30730478589420651</v>
+      </c>
+      <c r="M26" s="18">
         <f t="shared" si="3"/>
-        <v>-0.1475409836065574</v>
-      </c>
-      <c r="M26" t="s">
+        <v>0.26196473551637278</v>
+      </c>
+      <c r="N26" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.15617128463476065</v>
+      </c>
+      <c r="O26" s="1">
+        <f t="shared" si="5"/>
+        <v>-4.5340050377833729E-2</v>
+      </c>
+      <c r="P26" s="11">
+        <f t="shared" si="6"/>
+        <v>-0.29523809523809519</v>
+      </c>
+      <c r="Q26" s="1">
+        <f t="shared" si="7"/>
+        <v>-0.14754098360655732</v>
+      </c>
+      <c r="R26" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -2233,39 +2813,58 @@
       <c r="D27" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F27" s="11">
         <v>0.26700000000000002</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>4.7E-2</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>0.17699999999999999</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>-4.1000000000000002E-2</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="10">
         <f t="shared" si="0"/>
-        <v>-0.22000000000000003</v>
-      </c>
-      <c r="J27" s="1">
+        <v>0.57543103448275867</v>
+      </c>
+      <c r="K27" s="16">
         <f t="shared" si="1"/>
-        <v>-0.218</v>
-      </c>
-      <c r="K27" s="1">
+        <v>0.10129310344827586</v>
+      </c>
+      <c r="L27" s="16">
         <f t="shared" si="2"/>
+        <v>0.38146551724137928</v>
+      </c>
+      <c r="M27" s="18">
+        <f t="shared" si="3"/>
+        <v>-8.8362068965517238E-2</v>
+      </c>
+      <c r="N27" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.47413793103448282</v>
+      </c>
+      <c r="O27" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.46982758620689652</v>
+      </c>
+      <c r="P27" s="11">
+        <f t="shared" si="6"/>
         <v>-0.82397003745318353</v>
       </c>
-      <c r="L27" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q27" s="1">
+        <f t="shared" si="7"/>
         <v>-1.231638418079096</v>
       </c>
-      <c r="M27" t="s">
+      <c r="R27" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -2278,39 +2877,58 @@
       <c r="D28" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F28" s="11">
         <v>-4.3999999999999997E-2</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>-0.52800000000000002</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>1.4E-2</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>-4.9000000000000002E-2</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="10">
         <f t="shared" si="0"/>
-        <v>-0.48400000000000004</v>
-      </c>
-      <c r="J28" s="1">
-        <f t="shared" si="1"/>
-        <v>-6.3E-2</v>
-      </c>
-      <c r="K28" s="1">
-        <f>(F28-E28)/ABS(E28)</f>
+        <v>-0.31654676258992803</v>
+      </c>
+      <c r="K28" s="16">
+        <f>G28/$E28</f>
+        <v>-3.7985611510791366</v>
+      </c>
+      <c r="L28" s="16">
+        <f t="shared" si="2"/>
+        <v>0.10071942446043165</v>
+      </c>
+      <c r="M28" s="18">
+        <f t="shared" si="3"/>
+        <v>-0.35251798561151076</v>
+      </c>
+      <c r="N28" s="1">
+        <f>K28-J28</f>
+        <v>-3.4820143884892087</v>
+      </c>
+      <c r="O28" s="1">
+        <f>M28-L28</f>
+        <v>-0.4532374100719424</v>
+      </c>
+      <c r="P28" s="11">
+        <f>(K28-J28)/ABS(J28)</f>
         <v>-11.000000000000002</v>
       </c>
-      <c r="L28" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q28" s="1">
+        <f t="shared" si="7"/>
         <v>-4.5</v>
       </c>
-      <c r="M28" t="s">
+      <c r="R28" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
@@ -2323,39 +2941,58 @@
       <c r="D29" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="F29" s="11">
         <v>2.4E-2</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>-0.67100000000000004</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>-6.2E-2</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="10">
         <f t="shared" si="0"/>
-        <v>-0.69500000000000006</v>
-      </c>
-      <c r="J29" s="1">
+        <v>8.0267558528428096E-2</v>
+      </c>
+      <c r="K29" s="16">
         <f t="shared" si="1"/>
-        <v>-0.158</v>
-      </c>
-      <c r="K29" s="1">
+        <v>-2.2441471571906355</v>
+      </c>
+      <c r="L29" s="16">
         <f t="shared" si="2"/>
-        <v>-28.958333333333336</v>
-      </c>
-      <c r="L29" s="1">
+        <v>0.32107023411371238</v>
+      </c>
+      <c r="M29" s="18">
         <f t="shared" si="3"/>
+        <v>-0.20735785953177258</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="4"/>
+        <v>-2.3244147157190636</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.52842809364548493</v>
+      </c>
+      <c r="P29" s="11">
+        <f t="shared" si="6"/>
+        <v>-28.958333333333332</v>
+      </c>
+      <c r="Q29" s="1">
+        <f t="shared" si="7"/>
         <v>-1.6458333333333333</v>
       </c>
-      <c r="M29" t="s">
+      <c r="R29" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
@@ -2368,45 +3005,61 @@
       <c r="D30" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="F30" s="11">
         <v>0.16700000000000001</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>1.9E-2</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>0.112</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>0.05</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="10">
         <f t="shared" si="0"/>
-        <v>-0.14800000000000002</v>
-      </c>
-      <c r="J30" s="1">
+        <v>0.46778711484593843</v>
+      </c>
+      <c r="K30" s="16">
         <f t="shared" si="1"/>
-        <v>-6.2E-2</v>
-      </c>
-      <c r="K30" s="1">
+        <v>5.3221288515406161E-2</v>
+      </c>
+      <c r="L30" s="16">
         <f t="shared" si="2"/>
+        <v>0.31372549019607843</v>
+      </c>
+      <c r="M30" s="18">
+        <f t="shared" si="3"/>
+        <v>0.14005602240896359</v>
+      </c>
+      <c r="N30" s="1">
+        <f t="shared" si="4"/>
+        <v>-0.41456582633053229</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="5"/>
+        <v>-0.17366946778711484</v>
+      </c>
+      <c r="P30" s="11">
+        <f t="shared" si="6"/>
         <v>-0.88622754491017974</v>
       </c>
-      <c r="L30" s="1">
-        <f t="shared" si="3"/>
+      <c r="Q30" s="1">
+        <f t="shared" si="7"/>
         <v>-0.5535714285714286</v>
       </c>
-      <c r="M30" t="s">
+      <c r="R30" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="K28" formula="1"/>
+    <ignoredError sqref="P28" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>